<commit_message>
mise à jour des data
</commit_message>
<xml_diff>
--- a/1- ElIoT/Data/21-09-2025/Charge_utile_IoT data.xlsx
+++ b/1- ElIoT/Data/21-09-2025/Charge_utile_IoT data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flavien.serret\WORKSPACE\WorkshopNaasc\1- ElIoT\Data\21-09-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51793F5F-7D9F-4D1C-9283-0065B2602B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0125ABCC-E898-40B3-A941-261722EB6F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Température PCB (°C)</t>
   </si>
@@ -31,10 +31,7 @@
     <t>Gain</t>
   </si>
   <si>
-    <t>Température nominale (°C)</t>
-  </si>
-  <si>
-    <t>Gain nominal</t>
+    <t>Heure</t>
   </si>
 </sst>
 </file>
@@ -93,11 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +426,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,12 +438,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -456,6 +452,9 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="B2">
         <v>48.04</v>
       </c>
@@ -463,10 +462,13 @@
         <v>46.33</v>
       </c>
       <c r="D2">
-        <v>1.1459999999999999</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0.56956018518518514</v>
+      </c>
       <c r="B3">
         <v>49.58</v>
       </c>
@@ -474,16 +476,13 @@
         <v>56.08</v>
       </c>
       <c r="D3">
-        <v>1.0840000000000001</v>
-      </c>
-      <c r="E3">
-        <v>42.77</v>
-      </c>
-      <c r="F3">
-        <v>1.073</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0.56967592592592597</v>
+      </c>
       <c r="B4">
         <v>44.69</v>
       </c>
@@ -491,10 +490,13 @@
         <v>55.36</v>
       </c>
       <c r="D4">
-        <v>1.0309999999999999</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>0.56979166666666703</v>
+      </c>
       <c r="B5">
         <v>43.42</v>
       </c>
@@ -502,16 +504,13 @@
         <v>48.94</v>
       </c>
       <c r="D5">
-        <v>1.014</v>
-      </c>
-      <c r="E5">
-        <v>38.450000000000003</v>
-      </c>
-      <c r="F5">
-        <v>0.95099999999999996</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>0.56990740740740697</v>
+      </c>
       <c r="B6">
         <v>46.92</v>
       </c>
@@ -519,10 +518,13 @@
         <v>50.48</v>
       </c>
       <c r="D6">
-        <v>0.91800000000000004</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0.57002314814814803</v>
+      </c>
       <c r="B7">
         <v>43.9</v>
       </c>
@@ -530,10 +532,13 @@
         <v>47.99</v>
       </c>
       <c r="D7">
-        <v>1.167</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>0.57013888888888897</v>
+      </c>
       <c r="B8">
         <v>45.15</v>
       </c>
@@ -541,10 +546,13 @@
         <v>44.32</v>
       </c>
       <c r="D8">
-        <v>1.1779999999999999</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>0.57025462962962903</v>
+      </c>
       <c r="B9">
         <v>33.32</v>
       </c>
@@ -552,10 +560,13 @@
         <v>45.75</v>
       </c>
       <c r="D9">
-        <v>1.0289999999999999</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>0.57037037037036997</v>
+      </c>
       <c r="B10">
         <v>38.53</v>
       </c>
@@ -563,10 +574,13 @@
         <v>37.24</v>
       </c>
       <c r="D10">
-        <v>1.181</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>0.57048611111111103</v>
+      </c>
       <c r="B11">
         <v>39.03</v>
       </c>
@@ -574,10 +588,13 @@
         <v>45.29</v>
       </c>
       <c r="D11">
-        <v>0.97699999999999998</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>0.57060185185185197</v>
+      </c>
       <c r="B12">
         <v>45.53</v>
       </c>
@@ -585,10 +602,13 @@
         <v>42.18</v>
       </c>
       <c r="D12">
-        <v>1.1160000000000001</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>0.57071759259259203</v>
+      </c>
       <c r="B13">
         <v>52.46</v>
       </c>
@@ -596,10 +616,13 @@
         <v>52.42</v>
       </c>
       <c r="D13">
-        <v>0.83299999999999996</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>0.57083333333333297</v>
+      </c>
       <c r="B14">
         <v>40.020000000000003</v>
       </c>
@@ -607,10 +630,13 @@
         <v>50.95</v>
       </c>
       <c r="D14">
-        <v>0.95299999999999996</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>0.57094907407407403</v>
+      </c>
       <c r="B15">
         <v>48.21</v>
       </c>
@@ -618,10 +644,13 @@
         <v>48.89</v>
       </c>
       <c r="D15">
-        <v>1.0580000000000001</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>0.57106481481481497</v>
+      </c>
       <c r="B16">
         <v>46.36</v>
       </c>
@@ -629,16 +658,13 @@
         <v>42.63</v>
       </c>
       <c r="D16">
-        <v>0.86</v>
-      </c>
-      <c r="E16">
-        <v>40.81</v>
-      </c>
-      <c r="F16">
-        <v>1.0049999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>0.57118055555555503</v>
+      </c>
       <c r="B17">
         <v>47.31</v>
       </c>
@@ -646,10 +672,13 @@
         <v>58.89</v>
       </c>
       <c r="D17">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>0.57129629629629597</v>
+      </c>
       <c r="B18">
         <v>45.17</v>
       </c>
@@ -657,16 +686,13 @@
         <v>65.09</v>
       </c>
       <c r="D18">
-        <v>1.079</v>
-      </c>
-      <c r="E18">
-        <v>43.46</v>
-      </c>
-      <c r="F18">
-        <v>1.012</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>0.57141203703703702</v>
+      </c>
       <c r="B19">
         <v>49.28</v>
       </c>
@@ -674,10 +700,13 @@
         <v>38.1</v>
       </c>
       <c r="D19">
-        <v>0.81499999999999995</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>0.57152777777777697</v>
+      </c>
       <c r="B20">
         <v>46.79</v>
       </c>
@@ -685,10 +714,13 @@
         <v>40.46</v>
       </c>
       <c r="D20">
-        <v>0.95699999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0.57164351851851802</v>
+      </c>
       <c r="B21">
         <v>45.4</v>
       </c>
@@ -696,16 +728,13 @@
         <v>56.06</v>
       </c>
       <c r="D21">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="E21">
-        <v>44.25</v>
-      </c>
-      <c r="F21">
-        <v>1.0389999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>0.57175925925925897</v>
+      </c>
       <c r="B22">
         <v>40.409999999999997</v>
       </c>
@@ -713,10 +742,13 @@
         <v>46.71</v>
       </c>
       <c r="D22">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>0.57187500000000002</v>
+      </c>
       <c r="B23">
         <v>44.09</v>
       </c>
@@ -724,16 +756,13 @@
         <v>41.73</v>
       </c>
       <c r="D23">
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="E23">
-        <v>43.01</v>
-      </c>
-      <c r="F23">
-        <v>1.0640000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>0.57199074074073997</v>
+      </c>
       <c r="B24">
         <v>44.1</v>
       </c>
@@ -741,16 +770,13 @@
         <v>42.51</v>
       </c>
       <c r="D24">
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="E24">
-        <v>34.71</v>
-      </c>
-      <c r="F24">
-        <v>0.998</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>0.57210648148148102</v>
+      </c>
       <c r="B25">
         <v>55.26</v>
       </c>
@@ -758,10 +784,13 @@
         <v>42.25</v>
       </c>
       <c r="D25">
-        <v>1.016</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>0.57222222222222197</v>
+      </c>
       <c r="B26">
         <v>48.03</v>
       </c>
@@ -769,10 +798,13 @@
         <v>46.05</v>
       </c>
       <c r="D26">
-        <v>1.048</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>0.57233796296296202</v>
+      </c>
       <c r="B27">
         <v>42.54</v>
       </c>
@@ -780,16 +812,13 @@
         <v>64.03</v>
       </c>
       <c r="D27">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="E27">
-        <v>41.28</v>
-      </c>
-      <c r="F27">
-        <v>1.0760000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>0.57245370370370297</v>
+      </c>
       <c r="B28">
         <v>47.8</v>
       </c>
@@ -797,16 +826,13 @@
         <v>42.43</v>
       </c>
       <c r="D28">
-        <v>1.1439999999999999</v>
-      </c>
-      <c r="E28">
-        <v>38.97</v>
-      </c>
-      <c r="F28">
-        <v>1.0920000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>0.57256944444444402</v>
+      </c>
       <c r="B29">
         <v>40.090000000000003</v>
       </c>
@@ -814,10 +840,13 @@
         <v>49.98</v>
       </c>
       <c r="D29">
-        <v>1.0209999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>0.57268518518518496</v>
+      </c>
       <c r="B30">
         <v>47.89</v>
       </c>
@@ -825,16 +854,13 @@
         <v>46.29</v>
       </c>
       <c r="D30">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="E30">
-        <v>42.18</v>
-      </c>
-      <c r="F30">
-        <v>0.96199999999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>0.57280092592592502</v>
+      </c>
       <c r="B31">
         <v>50.73</v>
       </c>
@@ -842,16 +868,13 @@
         <v>57.35</v>
       </c>
       <c r="D31">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="E31">
-        <v>40.08</v>
-      </c>
-      <c r="F31">
-        <v>1.097</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>0.57291666666666596</v>
+      </c>
       <c r="B32">
         <v>51.08</v>
       </c>
@@ -859,10 +882,13 @@
         <v>54.47</v>
       </c>
       <c r="D32">
-        <v>1.1559999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>0.57303240740740702</v>
+      </c>
       <c r="B33">
         <v>47.69</v>
       </c>
@@ -870,16 +896,13 @@
         <v>57.06</v>
       </c>
       <c r="D33">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="E33">
-        <v>36.89</v>
-      </c>
-      <c r="F33">
-        <v>0.97199999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>0.57314814814814796</v>
+      </c>
       <c r="B34">
         <v>39.11</v>
       </c>
@@ -887,16 +910,13 @@
         <v>46.75</v>
       </c>
       <c r="D34">
-        <v>1.1020000000000001</v>
-      </c>
-      <c r="E34">
-        <v>41.06</v>
-      </c>
-      <c r="F34">
-        <v>0.90300000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>0.57326388888888802</v>
+      </c>
       <c r="B35">
         <v>43.4</v>
       </c>
@@ -904,10 +924,13 @@
         <v>54.09</v>
       </c>
       <c r="D35">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>0.57337962962962896</v>
+      </c>
       <c r="B36">
         <v>49.4</v>
       </c>
@@ -915,10 +938,13 @@
         <v>51.86</v>
       </c>
       <c r="D36">
-        <v>0.83299999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>0.57349537037037002</v>
+      </c>
       <c r="B37">
         <v>49.41</v>
       </c>
@@ -926,10 +952,13 @@
         <v>53.64</v>
       </c>
       <c r="D37">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>0.57361111111110996</v>
+      </c>
       <c r="B38">
         <v>44.83</v>
       </c>
@@ -937,10 +966,13 @@
         <v>49.78</v>
       </c>
       <c r="D38">
-        <v>0.86499999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>0.57372685185185102</v>
+      </c>
       <c r="B39">
         <v>48.17</v>
       </c>
@@ -948,10 +980,13 @@
         <v>36.799999999999997</v>
       </c>
       <c r="D39">
-        <v>1.0029999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>0.57384259259259196</v>
+      </c>
       <c r="B40">
         <v>56.79</v>
       </c>
@@ -959,10 +994,13 @@
         <v>53.79</v>
       </c>
       <c r="D40">
-        <v>1.1819999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>0.57395833333333302</v>
+      </c>
       <c r="B41">
         <v>44.18</v>
       </c>
@@ -970,10 +1008,13 @@
         <v>51.16</v>
       </c>
       <c r="D41">
-        <v>1.159</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>0.57407407407407296</v>
+      </c>
       <c r="B42">
         <v>52.67</v>
       </c>
@@ -981,10 +1022,13 @@
         <v>48.05</v>
       </c>
       <c r="D42">
-        <v>0.80800000000000005</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>0.57418981481481401</v>
+      </c>
       <c r="B43">
         <v>39.1</v>
       </c>
@@ -992,16 +1036,13 @@
         <v>42.97</v>
       </c>
       <c r="D43">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="E43">
-        <v>41.31</v>
-      </c>
-      <c r="F43">
-        <v>0.96499999999999997</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>0.57430555555555496</v>
+      </c>
       <c r="B44">
         <v>41.28</v>
       </c>
@@ -1009,16 +1050,13 @@
         <v>54.92</v>
       </c>
       <c r="D44">
-        <v>1.1459999999999999</v>
-      </c>
-      <c r="E44">
-        <v>37.43</v>
-      </c>
-      <c r="F44">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>0.57442129629629501</v>
+      </c>
       <c r="B45">
         <v>49.2</v>
       </c>
@@ -1026,10 +1064,13 @@
         <v>48.66</v>
       </c>
       <c r="D45">
-        <v>0.99199999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>0.57453703703703596</v>
+      </c>
       <c r="B46">
         <v>38.68</v>
       </c>
@@ -1037,10 +1078,13 @@
         <v>44.45</v>
       </c>
       <c r="D46">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>0.57465277777777701</v>
+      </c>
       <c r="B47">
         <v>42.66</v>
       </c>
@@ -1048,10 +1092,13 @@
         <v>49.23</v>
       </c>
       <c r="D47">
-        <v>1.0189999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>0.57476851851851796</v>
+      </c>
       <c r="B48">
         <v>54.42</v>
       </c>
@@ -1059,16 +1106,13 @@
         <v>48.78</v>
       </c>
       <c r="D48">
-        <v>0.88</v>
-      </c>
-      <c r="E48">
-        <v>39.67</v>
-      </c>
-      <c r="F48">
-        <v>1.024</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>0.57488425925925801</v>
+      </c>
       <c r="B49">
         <v>38.33</v>
       </c>
@@ -1076,10 +1120,13 @@
         <v>58.97</v>
       </c>
       <c r="D49">
-        <v>0.95699999999999996</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>0.57499999999999896</v>
+      </c>
       <c r="B50">
         <v>43.55</v>
       </c>
@@ -1087,16 +1134,13 @@
         <v>31.65</v>
       </c>
       <c r="D50">
-        <v>1.19</v>
-      </c>
-      <c r="E50">
-        <v>43.04</v>
-      </c>
-      <c r="F50">
-        <v>0.90500000000000003</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>0.57511574074074001</v>
+      </c>
       <c r="B51">
         <v>37.4</v>
       </c>
@@ -1104,16 +1148,13 @@
         <v>43.04</v>
       </c>
       <c r="D51">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="E51">
-        <v>37.5</v>
-      </c>
-      <c r="F51">
-        <v>0.99199999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>0.57523148148148096</v>
+      </c>
       <c r="B52">
         <v>50.15</v>
       </c>
@@ -1121,10 +1162,13 @@
         <v>39.19</v>
       </c>
       <c r="D52">
-        <v>1.1950000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>0.57534722222222101</v>
+      </c>
       <c r="B53">
         <v>46.35</v>
       </c>
@@ -1132,16 +1176,13 @@
         <v>49.62</v>
       </c>
       <c r="D53">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="E53">
-        <v>36.869999999999997</v>
-      </c>
-      <c r="F53">
-        <v>0.95699999999999996</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>0.57546296296296195</v>
+      </c>
       <c r="B54">
         <v>39.97</v>
       </c>
@@ -1149,10 +1190,13 @@
         <v>45.55</v>
       </c>
       <c r="D54">
-        <v>0.92700000000000005</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>0.57557870370370301</v>
+      </c>
       <c r="B55">
         <v>41.14</v>
       </c>
@@ -1160,10 +1204,13 @@
         <v>52.82</v>
       </c>
       <c r="D55">
-        <v>1.109</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>0.57569444444444295</v>
+      </c>
       <c r="B56">
         <v>40.22</v>
       </c>
@@ -1171,10 +1218,13 @@
         <v>50.3</v>
       </c>
       <c r="D56">
-        <v>0.91600000000000004</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>0.57581018518518401</v>
+      </c>
       <c r="B57">
         <v>48.12</v>
       </c>
@@ -1182,10 +1232,13 @@
         <v>54.27</v>
       </c>
       <c r="D57">
-        <v>1.101</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>0.57592592592592495</v>
+      </c>
       <c r="B58">
         <v>45.01</v>
       </c>
@@ -1193,16 +1246,13 @@
         <v>47.38</v>
       </c>
       <c r="D58">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="E58">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="F58">
-        <v>1.0760000000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>0.57604166666666601</v>
+      </c>
       <c r="B59">
         <v>47.9</v>
       </c>
@@ -1210,16 +1260,13 @@
         <v>63.82</v>
       </c>
       <c r="D59">
-        <v>0.82799999999999996</v>
-      </c>
-      <c r="E59">
-        <v>29.92</v>
-      </c>
-      <c r="F59">
-        <v>1.0980000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>0.57615740740740595</v>
+      </c>
       <c r="B60">
         <v>47.71</v>
       </c>
@@ -1227,16 +1274,13 @@
         <v>50.49</v>
       </c>
       <c r="D60">
-        <v>1.1990000000000001</v>
-      </c>
-      <c r="E60">
-        <v>36.979999999999997</v>
-      </c>
-      <c r="F60">
-        <v>1.0580000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>0.57627314814814701</v>
+      </c>
       <c r="B61">
         <v>44.19</v>
       </c>
@@ -1244,16 +1288,13 @@
         <v>51.81</v>
       </c>
       <c r="D61">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="E61">
-        <v>46.62</v>
-      </c>
-      <c r="F61">
-        <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>0.57638888888888795</v>
+      </c>
       <c r="B62">
         <v>37.119999999999997</v>
       </c>
@@ -1261,10 +1302,13 @@
         <v>42.83</v>
       </c>
       <c r="D62">
-        <v>1.1870000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>0.57650462962962801</v>
+      </c>
       <c r="B63">
         <v>46.83</v>
       </c>
@@ -1272,16 +1316,13 @@
         <v>51.44</v>
       </c>
       <c r="D63">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="E63">
-        <v>41.99</v>
-      </c>
-      <c r="F63">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>0.57662037037036895</v>
+      </c>
       <c r="B64">
         <v>38.33</v>
       </c>
@@ -1289,10 +1330,13 @@
         <v>43.31</v>
       </c>
       <c r="D64">
-        <v>0.83799999999999997</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>0.57673611111111001</v>
+      </c>
       <c r="B65">
         <v>42.3</v>
       </c>
@@ -1300,10 +1344,13 @@
         <v>57.95</v>
       </c>
       <c r="D65">
-        <v>0.94699999999999995</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>0.57685185185185095</v>
+      </c>
       <c r="B66">
         <v>46.3</v>
       </c>
@@ -1311,16 +1358,13 @@
         <v>62.58</v>
       </c>
       <c r="D66">
-        <v>0.86399999999999999</v>
-      </c>
-      <c r="E66">
-        <v>42.07</v>
-      </c>
-      <c r="F66">
-        <v>0.94199999999999995</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>0.57696759259259101</v>
+      </c>
       <c r="B67">
         <v>39.15</v>
       </c>
@@ -1328,10 +1372,13 @@
         <v>42.95</v>
       </c>
       <c r="D67">
-        <v>0.99099999999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>0.57708333333333195</v>
+      </c>
       <c r="B68">
         <v>47.15</v>
       </c>
@@ -1339,16 +1386,13 @@
         <v>41.42</v>
       </c>
       <c r="D68">
-        <v>0.97899999999999998</v>
-      </c>
-      <c r="E68">
-        <v>42.25</v>
-      </c>
-      <c r="F68">
-        <v>0.98699999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>0.577199074074073</v>
+      </c>
       <c r="B69">
         <v>42.45</v>
       </c>
@@ -1356,10 +1400,13 @@
         <v>63.23</v>
       </c>
       <c r="D69">
-        <v>1.0449999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>0.57731481481481395</v>
+      </c>
       <c r="B70">
         <v>41.57</v>
       </c>
@@ -1367,16 +1414,13 @@
         <v>54.06</v>
       </c>
       <c r="D70">
-        <v>1.018</v>
-      </c>
-      <c r="E70">
-        <v>35.36</v>
-      </c>
-      <c r="F70">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>0.577430555555554</v>
+      </c>
       <c r="B71">
         <v>45.97</v>
       </c>
@@ -1384,16 +1428,13 @@
         <v>47.72</v>
       </c>
       <c r="D71">
-        <v>1.085</v>
-      </c>
-      <c r="E71">
-        <v>38.82</v>
-      </c>
-      <c r="F71">
-        <v>1.012</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>0.57754629629629495</v>
+      </c>
       <c r="B72">
         <v>37.68</v>
       </c>
@@ -1401,16 +1442,13 @@
         <v>48.7</v>
       </c>
       <c r="D72">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="E72">
-        <v>41.87</v>
-      </c>
-      <c r="F72">
-        <v>1.0209999999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>0.577662037037036</v>
+      </c>
       <c r="B73">
         <v>55.23</v>
       </c>
@@ -1418,10 +1456,13 @@
         <v>32.35</v>
       </c>
       <c r="D73">
-        <v>0.98699999999999999</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>0.57777777777777595</v>
+      </c>
       <c r="B74">
         <v>33.85</v>
       </c>
@@ -1429,10 +1470,13 @@
         <v>50.72</v>
       </c>
       <c r="D74">
-        <v>0.85499999999999998</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>0.577893518518517</v>
+      </c>
       <c r="B75">
         <v>45.83</v>
       </c>
@@ -1440,10 +1484,13 @@
         <v>56.71</v>
       </c>
       <c r="D75">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>0.57800925925925795</v>
+      </c>
       <c r="B76">
         <v>32.47</v>
       </c>
@@ -1451,16 +1498,13 @@
         <v>59.61</v>
       </c>
       <c r="D76">
-        <v>1.06</v>
-      </c>
-      <c r="E76">
-        <v>39.4</v>
-      </c>
-      <c r="F76">
-        <v>1.0029999999999999</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>0.578124999999999</v>
+      </c>
       <c r="B77">
         <v>57.21</v>
       </c>
@@ -1468,10 +1512,13 @@
         <v>45.94</v>
       </c>
       <c r="D77">
-        <v>1.1160000000000001</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>0.57824074074073895</v>
+      </c>
       <c r="B78">
         <v>45.84</v>
       </c>
@@ -1479,10 +1526,13 @@
         <v>48.66</v>
       </c>
       <c r="D78">
-        <v>0.92800000000000005</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>0.57835648148148</v>
+      </c>
       <c r="B79">
         <v>42.48</v>
       </c>
@@ -1490,10 +1540,13 @@
         <v>55.89</v>
       </c>
       <c r="D79">
-        <v>1.0589999999999999</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>0.57847222222222106</v>
+      </c>
       <c r="B80">
         <v>34.04</v>
       </c>
@@ -1501,10 +1554,13 @@
         <v>52.17</v>
       </c>
       <c r="D80">
-        <v>1.119</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>0.578587962962961</v>
+      </c>
       <c r="B81">
         <v>43.82</v>
       </c>
@@ -1512,16 +1568,13 @@
         <v>50.35</v>
       </c>
       <c r="D81">
-        <v>1.0369999999999999</v>
-      </c>
-      <c r="E81">
-        <v>40.15</v>
-      </c>
-      <c r="F81">
-        <v>0.90200000000000002</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>0.57870370370370205</v>
+      </c>
       <c r="B82">
         <v>47.72</v>
       </c>
@@ -1529,16 +1582,13 @@
         <v>44.56</v>
       </c>
       <c r="D82">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="E82">
-        <v>39.03</v>
-      </c>
-      <c r="F82">
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>0.578819444444443</v>
+      </c>
       <c r="B83">
         <v>45.81</v>
       </c>
@@ -1546,16 +1596,13 @@
         <v>60.2</v>
       </c>
       <c r="D83">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="E83">
-        <v>46.03</v>
-      </c>
-      <c r="F83">
-        <v>0.98299999999999998</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>0.57893518518518405</v>
+      </c>
       <c r="B84">
         <v>44.51</v>
       </c>
@@ -1563,10 +1610,13 @@
         <v>54.41</v>
       </c>
       <c r="D84">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>0.579050925925924</v>
+      </c>
       <c r="B85">
         <v>39.24</v>
       </c>
@@ -1574,10 +1624,13 @@
         <v>52.49</v>
       </c>
       <c r="D85">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>0.57916666666666505</v>
+      </c>
       <c r="B86">
         <v>36.950000000000003</v>
       </c>
@@ -1585,10 +1638,13 @@
         <v>44.11</v>
       </c>
       <c r="D86">
-        <v>1.1879999999999999</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>0.579282407407406</v>
+      </c>
       <c r="B87">
         <v>49.79</v>
       </c>
@@ -1596,10 +1652,13 @@
         <v>48.28</v>
       </c>
       <c r="D87">
-        <v>0.89500000000000002</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>0.57939814814814605</v>
+      </c>
       <c r="B88">
         <v>55.5</v>
       </c>
@@ -1607,10 +1666,13 @@
         <v>48.4</v>
       </c>
       <c r="D88">
-        <v>0.98899999999999999</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>0.579513888888887</v>
+      </c>
       <c r="B89">
         <v>47.78</v>
       </c>
@@ -1618,10 +1680,13 @@
         <v>49.01</v>
       </c>
       <c r="D89">
-        <v>1.1970000000000001</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>0.57962962962962805</v>
+      </c>
       <c r="B90">
         <v>40.840000000000003</v>
       </c>
@@ -1629,10 +1694,13 @@
         <v>39.51</v>
       </c>
       <c r="D90">
-        <v>1.077</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>0.579745370370369</v>
+      </c>
       <c r="B91">
         <v>44.62</v>
       </c>
@@ -1640,10 +1708,13 @@
         <v>31.15</v>
       </c>
       <c r="D91">
-        <v>0.83599999999999997</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>0.57986111111110905</v>
+      </c>
       <c r="B92">
         <v>43.41</v>
       </c>
@@ -1651,10 +1722,13 @@
         <v>57.28</v>
       </c>
       <c r="D92">
-        <v>0.94299999999999995</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>0.57997685185184999</v>
+      </c>
       <c r="B93">
         <v>55.09</v>
       </c>
@@ -1662,16 +1736,13 @@
         <v>38.06</v>
       </c>
       <c r="D93">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="E93">
-        <v>45.6</v>
-      </c>
-      <c r="F93">
-        <v>1.0580000000000001</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>0.58009259259259105</v>
+      </c>
       <c r="B94">
         <v>47.56</v>
       </c>
@@ -1679,16 +1750,13 @@
         <v>53.27</v>
       </c>
       <c r="D94">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="E94">
-        <v>39.99</v>
-      </c>
-      <c r="F94">
-        <v>0.96199999999999997</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>0.58020833333333199</v>
+      </c>
       <c r="B95">
         <v>38.61</v>
       </c>
@@ -1696,10 +1764,13 @@
         <v>56.93</v>
       </c>
       <c r="D95">
-        <v>0.92800000000000005</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>0.58032407407407205</v>
+      </c>
       <c r="B96">
         <v>48.03</v>
       </c>
@@ -1707,10 +1778,13 @@
         <v>44.57</v>
       </c>
       <c r="D96">
-        <v>1.087</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>0.58043981481481299</v>
+      </c>
       <c r="B97">
         <v>41.81</v>
       </c>
@@ -1718,10 +1792,13 @@
         <v>52.57</v>
       </c>
       <c r="D97">
-        <v>1.1020000000000001</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>0.58055555555555405</v>
+      </c>
       <c r="B98">
         <v>42.73</v>
       </c>
@@ -1729,16 +1806,13 @@
         <v>64.88</v>
       </c>
       <c r="D98">
-        <v>1.101</v>
-      </c>
-      <c r="E98">
-        <v>40.659999999999997</v>
-      </c>
-      <c r="F98">
-        <v>1.0720000000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>0.58067129629629399</v>
+      </c>
       <c r="B99">
         <v>38.82</v>
       </c>
@@ -1746,10 +1820,13 @@
         <v>49.04</v>
       </c>
       <c r="D99">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>0.58078703703703505</v>
+      </c>
       <c r="B100">
         <v>44.37</v>
       </c>
@@ -1757,10 +1834,13 @@
         <v>36.58</v>
       </c>
       <c r="D100">
-        <v>1.137</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>0.58090277777777599</v>
+      </c>
       <c r="B101">
         <v>41.11</v>
       </c>
@@ -1768,13 +1848,7 @@
         <v>50.21</v>
       </c>
       <c r="D101">
-        <v>1.044</v>
-      </c>
-      <c r="E101">
-        <v>37.18</v>
-      </c>
-      <c r="F101">
-        <v>0.93500000000000005</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>